<commit_message>
update the Navigation Smoke scripts
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Provana\Automation\IPACS\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zan\IPACS_Smoke\IPACS\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6403445-283C-4F7B-A6F7-8B85C7ED5850}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D298B511-3DF1-488A-BC7C-1DEBB22FAB71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ipacs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <t>https://ic247gateway.iconnect247.com/IConnectGatewayV3QA/Account/Login</t>
   </si>
   <si>
-    <t>https://trail.provanaipacs.com/</t>
+    <t>https://trial.provanaipacs.com/</t>
   </si>
 </sst>
 </file>
@@ -397,13 +397,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="33.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,13 +419,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
     </row>
   </sheetData>
@@ -445,13 +445,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="2" max="2" width="61.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D6E0DF56-E798-4E99-AC48-7336BB8CD52F}"/>

</xml_diff>